<commit_message>
added individual vins for the ss tests.
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NewVIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NewVIN_UT_SS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8328"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -630,34 +630,34 @@
   <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.5546875" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" customWidth="1"/>
-    <col min="21" max="21" width="22.88671875" customWidth="1"/>
-    <col min="23" max="23" width="22.21875" customWidth="1"/>
-    <col min="24" max="24" width="20.88671875" customWidth="1"/>
-    <col min="25" max="25" width="34.77734375" customWidth="1"/>
-    <col min="26" max="26" width="5.88671875" customWidth="1"/>
-    <col min="27" max="27" width="16.21875" customWidth="1"/>
-    <col min="28" max="29" width="13.77734375" customWidth="1"/>
-    <col min="35" max="35" width="19.88671875" customWidth="1"/>
-    <col min="36" max="36" width="21.88671875" customWidth="1"/>
-    <col min="38" max="38" width="20.88671875" customWidth="1"/>
+    <col min="12" max="12" width="24.5703125" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="21" max="21" width="22.85546875" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" customWidth="1"/>
+    <col min="24" max="24" width="20.85546875" customWidth="1"/>
+    <col min="25" max="25" width="34.7109375" customWidth="1"/>
+    <col min="26" max="26" width="5.85546875" customWidth="1"/>
+    <col min="27" max="27" width="16.28515625" customWidth="1"/>
+    <col min="28" max="29" width="13.7109375" customWidth="1"/>
+    <col min="35" max="35" width="19.85546875" customWidth="1"/>
+    <col min="36" max="36" width="21.85546875" customWidth="1"/>
+    <col min="38" max="38" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,7 +773,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -889,7 +889,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
NewVIN_UT_SS.xlsx fixed vin version TestVINUpload small cleanup
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NewVIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NewVIN_UT_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSAA\CODE\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="73">
   <si>
     <t>VIN</t>
   </si>
@@ -140,9 +140,6 @@
     <t>B-IMMOBILIZER/KEYLSS ENTRY/ALARM</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>Gt</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>invalidVIN</t>
   </si>
   <si>
@@ -197,10 +191,58 @@
     <t>TOYOTA</t>
   </si>
   <si>
-    <t>SYMBOL_2000</t>
-  </si>
-  <si>
     <t>AAAKN3DD&amp;E</t>
+  </si>
+  <si>
+    <t>BI001</t>
+  </si>
+  <si>
+    <t>PD001</t>
+  </si>
+  <si>
+    <t>UM001</t>
+  </si>
+  <si>
+    <t>MP001</t>
+  </si>
+  <si>
+    <t>BI002</t>
+  </si>
+  <si>
+    <t>PD002</t>
+  </si>
+  <si>
+    <t>UM002</t>
+  </si>
+  <si>
+    <t>MP002</t>
+  </si>
+  <si>
+    <t>BI003</t>
+  </si>
+  <si>
+    <t>BI004</t>
+  </si>
+  <si>
+    <t>PD003</t>
+  </si>
+  <si>
+    <t>PD004</t>
+  </si>
+  <si>
+    <t>UM003</t>
+  </si>
+  <si>
+    <t>UM004</t>
+  </si>
+  <si>
+    <t>MP003</t>
+  </si>
+  <si>
+    <t>MP004</t>
+  </si>
+  <si>
+    <t>SYMBOL_2017</t>
   </si>
 </sst>
 </file>
@@ -546,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AE17" sqref="AE17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,48 +702,48 @@
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3">
         <v>2018</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>28</v>
@@ -713,19 +755,19 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O2" s="3">
         <v>8</v>
@@ -767,51 +809,51 @@
         <v>42</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="AG2" s="3">
         <v>20010101</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C3" s="3">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>28</v>
@@ -823,19 +865,19 @@
         <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O3" s="3">
         <v>8</v>
@@ -877,51 +919,51 @@
         <v>42</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="AG3" s="3">
         <v>20000101</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C4" s="3">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>28</v>
@@ -933,19 +975,19 @@
         <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O4" s="3">
         <v>8</v>
@@ -987,51 +1029,51 @@
         <v>42</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="AG4" s="3">
         <v>20150101</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C5" s="3">
         <v>2018</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>28</v>
@@ -1043,19 +1085,19 @@
         <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O5" s="3">
         <v>8</v>
@@ -1097,31 +1139,31 @@
         <v>42</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="AG5" s="3">
         <v>20190101</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pas533_newVinAdded small cleaning NewVIN_UT_SS.xlsx : VIN version changed to SYMBOL_2017
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NewVIN_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NewVIN_UT_SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSAA\CODE\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="73">
   <si>
     <t>VIN</t>
   </si>
@@ -140,9 +140,6 @@
     <t>B-IMMOBILIZER/KEYLSS ENTRY/ALARM</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>Gt</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>invalidVIN</t>
   </si>
   <si>
@@ -197,10 +191,58 @@
     <t>TOYOTA</t>
   </si>
   <si>
-    <t>SYMBOL_2000</t>
-  </si>
-  <si>
     <t>AAAKN3DD&amp;E</t>
+  </si>
+  <si>
+    <t>BI001</t>
+  </si>
+  <si>
+    <t>PD001</t>
+  </si>
+  <si>
+    <t>UM001</t>
+  </si>
+  <si>
+    <t>MP001</t>
+  </si>
+  <si>
+    <t>BI002</t>
+  </si>
+  <si>
+    <t>PD002</t>
+  </si>
+  <si>
+    <t>UM002</t>
+  </si>
+  <si>
+    <t>MP002</t>
+  </si>
+  <si>
+    <t>BI003</t>
+  </si>
+  <si>
+    <t>BI004</t>
+  </si>
+  <si>
+    <t>PD003</t>
+  </si>
+  <si>
+    <t>PD004</t>
+  </si>
+  <si>
+    <t>UM003</t>
+  </si>
+  <si>
+    <t>UM004</t>
+  </si>
+  <si>
+    <t>MP003</t>
+  </si>
+  <si>
+    <t>MP004</t>
+  </si>
+  <si>
+    <t>SYMBOL_2017</t>
   </si>
 </sst>
 </file>
@@ -546,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AE17" sqref="AE17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,48 +702,48 @@
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3">
         <v>2018</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>28</v>
@@ -713,19 +755,19 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O2" s="3">
         <v>8</v>
@@ -767,51 +809,51 @@
         <v>42</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="AG2" s="3">
         <v>20010101</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C3" s="3">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>28</v>
@@ -823,19 +865,19 @@
         <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O3" s="3">
         <v>8</v>
@@ -877,51 +919,51 @@
         <v>42</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="AD3" s="3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="AG3" s="3">
         <v>20000101</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C4" s="3">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>28</v>
@@ -933,19 +975,19 @@
         <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O4" s="3">
         <v>8</v>
@@ -987,51 +1029,51 @@
         <v>42</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="AG4" s="3">
         <v>20150101</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C5" s="3">
         <v>2018</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>28</v>
@@ -1043,19 +1085,19 @@
         <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O5" s="3">
         <v>8</v>
@@ -1097,31 +1139,31 @@
         <v>42</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC5" s="3" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="AD5" s="3" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="AF5" s="3" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="AG5" s="3">
         <v>20190101</v>
       </c>
       <c r="AH5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>